<commit_message>
allows to input dividend as a list
</commit_message>
<xml_diff>
--- a/company_template.xlsx
+++ b/company_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z003eb4h\Desktop\codes\GitHub\finagle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC6D433-1DBB-4DD7-BE27-7AA61FB938CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D156EDD-7C96-44A9-94F2-29B52259FFD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="report" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="67">
   <si>
     <t>Ticker Symbol</t>
   </si>
@@ -99,12 +99,6 @@
   </si>
   <si>
     <t>FCFE</t>
-  </si>
-  <si>
-    <t>Equity, Intrisic Value</t>
-  </si>
-  <si>
-    <t>PV of FCFE</t>
   </si>
   <si>
     <t>FCFF</t>
@@ -200,22 +194,10 @@
     <t>Cash Generated</t>
   </si>
   <si>
-    <t>Potential Buyback</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
     <t>shares</t>
   </si>
   <si>
     <t>price</t>
-  </si>
-  <si>
-    <t>Implied multiple</t>
-  </si>
-  <si>
-    <t>IV per share incl. buybacks</t>
   </si>
   <si>
     <t>MnA</t>
@@ -226,6 +208,33 @@
   <si>
     <t>Cash (on balance-sheet)</t>
   </si>
+  <si>
+    <t>Shares for DDM model</t>
+  </si>
+  <si>
+    <t>Buyback in DDM model</t>
+  </si>
+  <si>
+    <t>Dividend in DDM model</t>
+  </si>
+  <si>
+    <t>IV per share DDM model</t>
+  </si>
+  <si>
+    <t>dividend</t>
+  </si>
+  <si>
+    <t>buybacks</t>
+  </si>
+  <si>
+    <t>Price for DDM model</t>
+  </si>
+  <si>
+    <t>Implied multiple for DDM model</t>
+  </si>
+  <si>
+    <t>value_per_share_DDM</t>
+  </si>
 </sst>
 </file>
 
@@ -235,10 +244,10 @@
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.0_-;\-&quot;$&quot;* #,##0.0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.0"/>
-    <numFmt numFmtId="168" formatCode="0.0%"/>
-    <numFmt numFmtId="169" formatCode="0.0"/>
-    <numFmt numFmtId="170" formatCode="#,##0.0"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.0"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
+    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="169" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -354,11 +363,11 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -366,8 +375,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -380,7 +389,17 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Pandas" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -782,31 +801,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:BF57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47:AY47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="27.109375" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="7" width="10.77734375" style="5" customWidth="1"/>
     <col min="8" max="51" width="10.33203125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:2" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="9"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:2" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="10"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:2" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="9"/>
@@ -844,19 +863,19 @@
     </row>
     <row r="11" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B11" s="16"/>
     </row>
     <row r="12" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B12" s="16"/>
     </row>
     <row r="13" spans="1:2" s="5" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B13" s="16"/>
     </row>
@@ -886,7 +905,7 @@
     </row>
     <row r="17" spans="1:58" s="5" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B17" s="14"/>
     </row>
@@ -2543,7 +2562,7 @@
     </row>
     <row r="27" spans="1:58" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B27" s="12" t="e">
         <f>VLOOKUP(keys!$A$25,'raw data'!$A$1:$AY$39,COLUMN(B27),FALSE)</f>
@@ -2955,8 +2974,8 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="29" spans="1:58" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:58" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B29" s="12" t="e">
@@ -3578,263 +3597,413 @@
     </row>
     <row r="33" spans="1:51" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="B33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(B32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(B32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="C33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(C32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(C32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(D32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(D32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="E33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(E32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(E32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(F32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(F32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="G33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(G32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(G32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="H33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(H32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(H32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="I33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(I32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(I32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="J33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(J32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(J32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="K33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(K32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(K32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(L32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(L32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="M33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(M32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(M32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="N33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(N32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(N32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="O33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(O32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(O32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="P33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(P32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(P32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="Q33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(Q32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(Q32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="R33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(R32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(R32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="S33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(S32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(S32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="T33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(T32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(T32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="U33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(U32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(U32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="V33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(V32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(V32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="W33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(W32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(W32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="X33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(X32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(X32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="Y33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(Y32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(Y32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="Z33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(Z32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(Z32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="AA33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(AA32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(AA32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="AB33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(AB32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(AB32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="AC33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(AC32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(AC32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="AD33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(AD32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(AD32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="AE33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(AE32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(AE32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="AF33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(AF32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(AF32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="AG33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(AG32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(AG32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="AH33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(AH32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(AH32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="AI33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(AI32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(AI32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="AJ33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(AJ32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(AJ32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="AK33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(AK32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(AK32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="AL33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(AL32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(AL32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="AM33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(AM32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(AM32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="AN33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(AN32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(AN32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="AO33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(AO32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(AO32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="AP33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(AP32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(AP32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="AQ33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(AQ32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(AQ32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="AR33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(AR32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(AR32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="AS33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(AS32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(AS32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="AT33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(AT32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(AT32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="AU33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(AU32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(AU32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="AV33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(AV32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(AV32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="AW33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(AW32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(AW32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="AX33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(AX32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(AX32),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="AY33" s="12" t="e">
-        <f>VLOOKUP(keys!$A$18,'raw data'!$A$1:$AY$39,COLUMN(AY32),FALSE)</f>
+        <f>VLOOKUP(keys!$A$28,'raw data'!$A$1:$AY$39,COLUMN(AY32),FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="34" spans="1:51" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="12"/>
-      <c r="J34" s="12"/>
-      <c r="K34" s="12"/>
-      <c r="L34" s="12"/>
-      <c r="M34" s="12"/>
-      <c r="N34" s="12"/>
-      <c r="O34" s="12"/>
-      <c r="P34" s="12"/>
-      <c r="Q34" s="12"/>
-      <c r="R34" s="12"/>
-      <c r="S34" s="12"/>
-      <c r="T34" s="12"/>
-      <c r="U34" s="12"/>
-      <c r="V34" s="12"/>
-      <c r="W34" s="12"/>
-      <c r="X34" s="12"/>
-      <c r="Y34" s="12"/>
-      <c r="Z34" s="12"/>
-      <c r="AA34" s="12"/>
-      <c r="AB34" s="12"/>
-      <c r="AC34" s="12"/>
-      <c r="AD34" s="12"/>
-      <c r="AE34" s="12"/>
-      <c r="AF34" s="12"/>
-      <c r="AG34" s="12"/>
-      <c r="AH34" s="12"/>
-      <c r="AI34" s="12"/>
-      <c r="AJ34" s="12"/>
-      <c r="AK34" s="12"/>
-      <c r="AL34" s="12"/>
-      <c r="AM34" s="12"/>
-      <c r="AN34" s="12"/>
-      <c r="AO34" s="12"/>
-      <c r="AP34" s="12"/>
-      <c r="AQ34" s="12"/>
-      <c r="AR34" s="12"/>
-      <c r="AS34" s="12"/>
-      <c r="AT34" s="12"/>
-      <c r="AU34" s="12"/>
-      <c r="AV34" s="12"/>
-      <c r="AW34" s="12"/>
-      <c r="AX34" s="12"/>
-      <c r="AY34" s="12"/>
+        <v>60</v>
+      </c>
+      <c r="B34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(B33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(C33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(D33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(E33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(F33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(G33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(H33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(I33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(J33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(K33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="L34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(L33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(M33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(N33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(O33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(P33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(Q33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(R33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="S34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(S33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="T34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(T33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(U33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="V34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(V33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="W34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(W33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="X34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(X33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Y34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(Y33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Z34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(Z33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AA34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(AA33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AB34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(AB33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AC34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(AC33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AD34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(AD33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AE34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(AE33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AF34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(AF33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AG34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(AG33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AH34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(AH33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AI34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(AI33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AJ34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(AJ33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AK34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(AK33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AL34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(AL33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AM34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(AM33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AN34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(AN33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AO34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(AO33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AP34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(AP33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AQ34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(AQ33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AR34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(AR33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AS34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(AS33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AT34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(AT33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AU34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(AU33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AV34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(AV33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AW34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(AW33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AX34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(AX33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AY34" s="12" t="e">
+        <f>VLOOKUP(keys!$A$27,'raw data'!$A$1:$AY$39,COLUMN(AY33),FALSE)</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="35" spans="1:51" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
@@ -3891,7 +4060,7 @@
     </row>
     <row r="36" spans="1:51" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B36" s="12" t="e">
         <f>VLOOKUP(keys!$A$12,'raw data'!$A$1:$AY$39,COLUMN(B35),FALSE)</f>
@@ -4096,7 +4265,7 @@
     </row>
     <row r="37" spans="1:51" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B37" s="12" t="e">
         <f>VLOOKUP(keys!$A$21,'raw data'!$A$1:$AY$39,COLUMN(B36),FALSE)</f>
@@ -4301,7 +4470,7 @@
     </row>
     <row r="38" spans="1:51" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
@@ -4409,7 +4578,7 @@
     </row>
     <row r="40" spans="1:51" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B40" s="12" t="e">
         <f>VLOOKUP(keys!$A$6,'raw data'!$A$1:$AY$39,COLUMN(B39),FALSE)</f>
@@ -4614,7 +4783,7 @@
     </row>
     <row r="41" spans="1:51" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B41" s="12" t="e">
         <f>VLOOKUP(keys!$A$19,'raw data'!$A$1:$AY$39,COLUMN(B40),FALSE)</f>
@@ -4819,7 +4988,7 @@
     </row>
     <row r="42" spans="1:51" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B42" s="6" t="e">
         <f>VLOOKUP(keys!$A$20,'raw data'!$A$1:$AY$39,COLUMN(B41),FALSE)</f>
@@ -5229,7 +5398,7 @@
     </row>
     <row r="44" spans="1:51" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B44" s="13" t="e">
         <f>VLOOKUP(keys!$A$8,'raw data'!$A$1:$AY$39,COLUMN(B43),FALSE)</f>
@@ -5434,7 +5603,7 @@
     </row>
     <row r="45" spans="1:51" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B45" s="13" t="e">
         <f>VLOOKUP(keys!$A$26,'raw data'!$A$1:$AY$39,COLUMN(B44),FALSE)</f>
@@ -5842,18 +6011,213 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="47" spans="1:51" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="18"/>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
+    <row r="47" spans="1:51" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(B45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(C45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(D45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(E45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(F45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(G45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(H45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(I45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(J45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(K45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="L47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(L45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(M45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(N45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(O45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(P45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(Q45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(R45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="S47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(S45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="T47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(T45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(U45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="V47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(V45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="W47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(W45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="X47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(X45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Y47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(Y45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Z47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(Z45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AA47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(AA45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AB47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(AB45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AC47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(AC45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AD47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(AD45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AE47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(AE45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AF47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(AF45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AG47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(AG45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AH47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(AH45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AI47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(AI45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AJ47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(AJ45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AK47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(AK45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AL47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(AL45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AM47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(AM45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AN47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(AN45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AO47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(AO45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AP47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(AP45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AQ47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(AQ45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AR47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(AR45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AS47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(AS45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AT47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(AT45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AU47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(AU45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AV47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(AV45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AW47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(AW45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AX47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(AX45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AY47" s="13" t="e">
+        <f>VLOOKUP(keys!$A$29,'raw data'!$A$1:$AY$39,COLUMN(AY45),FALSE)</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="48" spans="1:51" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="20" t="s">
-        <v>55</v>
-      </c>
+      <c r="A48" s="20"/>
       <c r="B48" s="19"/>
       <c r="C48" s="18"/>
       <c r="D48" s="18"/>
@@ -5862,7 +6226,7 @@
     </row>
     <row r="49" spans="1:58" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="20" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="B49" s="22" t="e">
         <f>VLOOKUP(keys!$A$23,'raw data'!$A$1:$AY$39,COLUMN(B48),FALSE)</f>
@@ -6067,7 +6431,7 @@
     </row>
     <row r="50" spans="1:58" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="20" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="B50" s="13" t="e">
         <f>VLOOKUP(keys!$A$24,'raw data'!$A$1:$AY$39,COLUMN(B49),FALSE)</f>
@@ -6272,7 +6636,7 @@
     </row>
     <row r="51" spans="1:58" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="20" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B51" s="21" t="e">
         <f>(B49*B50+B40-B44)/C20</f>
@@ -6488,69 +6852,79 @@
     <row r="56" spans="1:58" ht="13.8" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="57" spans="1:58" ht="13.8" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="B31:AY43 B20:AY26 B28:AY29 B27:BC27">
-    <cfRule type="expression" dxfId="12" priority="20">
+  <conditionalFormatting sqref="B20:AY26 B28:AY29 B27:BC27 B31:AY43">
+    <cfRule type="expression" dxfId="14" priority="22">
       <formula>B$19&lt;0.1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B19:AY26 B28:AY43 B27:BC27">
-    <cfRule type="expression" dxfId="11" priority="18">
+  <conditionalFormatting sqref="B19:AY26 B27:BC27 B28:AY43">
+    <cfRule type="expression" dxfId="13" priority="20">
       <formula>ISNA(B19)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:AY19">
-    <cfRule type="expression" dxfId="10" priority="17">
+    <cfRule type="expression" dxfId="12" priority="19">
       <formula>B$19&lt;0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44:AY44">
+    <cfRule type="expression" dxfId="11" priority="14">
+      <formula>B$19&lt;0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B44:AY44">
+    <cfRule type="expression" dxfId="10" priority="13">
+      <formula>ISNA(B44)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B46:AY46">
     <cfRule type="expression" dxfId="9" priority="12">
       <formula>B$19&lt;0.1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B44:AY44">
+  <conditionalFormatting sqref="B46:AY46">
     <cfRule type="expression" dxfId="8" priority="11">
-      <formula>ISNA(B44)</formula>
+      <formula>ISNA(B46)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B46:AY46">
+  <conditionalFormatting sqref="B49:AY49">
     <cfRule type="expression" dxfId="7" priority="10">
       <formula>B$19&lt;0.1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B46:AY46">
+  <conditionalFormatting sqref="B49:AY49">
     <cfRule type="expression" dxfId="6" priority="9">
-      <formula>ISNA(B46)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B49:AY49">
-    <cfRule type="expression" dxfId="5" priority="8">
-      <formula>B$19&lt;0.1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B49:AY49">
-    <cfRule type="expression" dxfId="4" priority="7">
       <formula>ISNA(B49)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B50:AY50">
+    <cfRule type="expression" dxfId="5" priority="6">
+      <formula>B$19&lt;0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B50:AY50">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>ISNA(B50)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B45:AY45">
     <cfRule type="expression" dxfId="3" priority="4">
       <formula>B$19&lt;0.1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B50:AY50">
+  <conditionalFormatting sqref="B45:AY45">
     <cfRule type="expression" dxfId="2" priority="3">
-      <formula>ISNA(B50)</formula>
+      <formula>ISNA(B45)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B45:AY45">
+  <conditionalFormatting sqref="B47:AY47">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>B$19&lt;0.1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B45:AY45">
+  <conditionalFormatting sqref="B47:AY47">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>ISNA(B45)</formula>
+      <formula>ISNA(B47)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6567,7 +6941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -6585,10 +6959,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:A26"/>
+  <dimension ref="A1:A29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:A26"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6598,72 +6972,72 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
@@ -6673,57 +7047,72 @@
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>